<commit_message>
commit nav + sect
</commit_message>
<xml_diff>
--- a/inst/app/www/data_dashboardr.xlsx
+++ b/inst/app/www/data_dashboardr.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="59">
   <si>
     <t>id</t>
   </si>
@@ -158,37 +158,49 @@
     <t>sect_footer_bgcolor</t>
   </si>
   <si>
+    <t>sect_tlp_msg</t>
+  </si>
+  <si>
+    <t>sect_tlp_color</t>
+  </si>
+  <si>
+    <t>sect_tlp_position</t>
+  </si>
+  <si>
+    <t>%r% tagList(icon("cog"),tags$span("Titre 2"))</t>
+  </si>
+  <si>
+    <t>Evolution temporelle du COVID-19</t>
+  </si>
+  <si>
+    <t>sect_title_color</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>nav_title</t>
+  </si>
+  <si>
+    <t>nav_icon_name</t>
+  </si>
+  <si>
+    <t>nav_icon_lib</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>titre1</t>
+  </si>
+  <si>
+    <t>titre2</t>
+  </si>
+  <si>
     <t>primary</t>
   </si>
   <si>
-    <t>danger</t>
-  </si>
-  <si>
-    <t>sect_tlp_msg</t>
-  </si>
-  <si>
-    <t>sect_tlp_color</t>
-  </si>
-  <si>
-    <t>sect_tlp_position</t>
-  </si>
-  <si>
-    <t>essai</t>
-  </si>
-  <si>
-    <t>%r% tagList(icon("cog"),tags$span("Titre 2"))</t>
-  </si>
-  <si>
-    <t>reeee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">essai2 dfsdfsdf s fds dfs fs sdf sf sdf sdf sd fsd f sdf sdf sdf sdf sdf sd fsd f sdf sdf sdvxc v xcv xv xcv xcv xc vxcvxcvxcv </t>
-  </si>
-  <si>
-    <t>Evolution temporelle du COVID-19</t>
-  </si>
-  <si>
-    <t>warning</t>
+    <t>yeaaaahhhhhh !</t>
   </si>
 </sst>
 </file>
@@ -509,32 +521,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U8"/>
+  <dimension ref="A1:Y8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="7" width="11.5546875" style="1"/>
-    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="12.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18" style="1" customWidth="1"/>
-    <col min="14" max="14" width="31.21875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.5546875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.5546875" style="1" customWidth="1"/>
-    <col min="20" max="20" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="11.5546875" style="1"/>
+    <col min="1" max="10" width="11.5546875" style="1"/>
+    <col min="11" max="11" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="12.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18" style="1" customWidth="1"/>
+    <col min="17" max="17" width="31.21875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.5546875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.6640625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="17.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.5546875" style="1" customWidth="1"/>
+    <col min="24" max="24" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -551,55 +564,67 @@
         <v>20</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="U1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="W1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>48</v>
-      </c>
     </row>
-    <row r="2" spans="1:21" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -615,41 +640,35 @@
       <c r="E2" s="1">
         <v>1</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="1">
+      <c r="K2" s="1">
         <v>12</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="N2" s="1" t="s">
+      <c r="P2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="R2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="P2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="T2" s="1" t="s">
-        <v>45</v>
+        <v>57</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -665,35 +684,26 @@
       <c r="E3" s="1">
         <v>2</v>
       </c>
-      <c r="J3" s="1">
+      <c r="M3" s="1">
         <v>6</v>
       </c>
-      <c r="K3" s="1">
+      <c r="N3" s="1">
         <v>6</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="P3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="O3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="P3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>44</v>
-      </c>
     </row>
-    <row r="4" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -710,37 +720,37 @@
         <v>3</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="1">
+      <c r="M4" s="1">
         <v>6</v>
       </c>
-      <c r="K4" s="1">
+      <c r="N4" s="1">
         <v>6</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="R4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="S4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="P4" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>44</v>
-      </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -756,32 +766,32 @@
       <c r="E5" s="1">
         <v>3</v>
       </c>
-      <c r="J5" s="1">
+      <c r="F5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M5" s="1">
         <v>6</v>
       </c>
-      <c r="K5" s="1">
+      <c r="N5" s="1">
         <v>6</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="Q5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="R5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="S5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="P5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>44</v>
-      </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -797,35 +807,29 @@
       <c r="E6" s="1">
         <v>1</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="1">
+      <c r="M6" s="1">
         <v>6</v>
       </c>
-      <c r="K6" s="1">
+      <c r="N6" s="1">
         <v>4</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="P6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="R6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="S6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="S6" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>44</v>
-      </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -841,32 +845,26 @@
       <c r="E7" s="1">
         <v>2</v>
       </c>
-      <c r="J7" s="1">
+      <c r="M7" s="1">
         <v>6</v>
       </c>
-      <c r="K7" s="1">
+      <c r="N7" s="1">
         <v>4</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="P7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="Q7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="R7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="S7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="S7" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="T7" s="1" t="s">
-        <v>44</v>
-      </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -882,32 +880,26 @@
       <c r="E8" s="1">
         <v>3</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="1">
+      <c r="M8" s="1">
         <v>6</v>
       </c>
-      <c r="K8" s="1">
+      <c r="N8" s="1">
         <v>4</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="Q8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="R8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="S8" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="S8" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="T8" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>